<commit_message>
initial refactor to OOP
</commit_message>
<xml_diff>
--- a/outputs/compliance_results_2025-10-24.xlsx
+++ b/outputs/compliance_results_2025-10-24.xlsx
@@ -599,7 +599,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -713,7 +713,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -1267,7 +1267,7 @@
     <col width="14" customWidth="1" min="8" max="8"/>
     <col width="30" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
     <col width="42" customWidth="1" min="12" max="12"/>
     <col width="50" customWidth="1" min="13" max="13"/>
     <col width="50" customWidth="1" min="14" max="14"/>
@@ -1418,16 +1418,16 @@
         <v/>
       </c>
       <c r="H2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1506</v>
+        <v>0.1512</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>AMGN, MCD, MCD, MCD, MCD, MCD, MCD, MCD, MCD, MCD, MCD, MCD, MCD, MRK, MRK, MRK, MRK, MRK, MRK, MRK, MRK, MCD, MCD, AMGN, MCD, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, KO, MCD, MCD, MCD, MRK, MRK, MRK, MRK, PG, PG, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, VZ, PG, PG, PG, PG, MRK, MRK, MRK, MRK, MRK, MRK, PG, PG, PG, PG, PG, PG, PG, PG, PG, PG, PG, PG, KO, KO, JNJ, CVX, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CSCO, CVX, CVX, CVX, CVX, CVX, CVX, CVX, CSCO, CSCO, CSCO, AMGN, AMGN, AMGN, AMGN, AMGN, AMGN, AMGN, AMGN, AMGN, AMGN, CSCO, AMGN, AMGN, AMGN, AMGN, AMGN, AMGN, CSCO, CSCO, CVX, CVX, JNJ, CVX, IBM, IBM, IBM, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, JNJ, IBM, IBM, IBM, IBM, CVX, CVX, CVX, CVX, CVX, CVX, CVX, IBM, IBM, IBM, IBM, IBM, IBM, IBM, IBM, IBM, IBM, IBM, VZ</t>
+          <t>AMGN, AMGN, VZ, VZ, PG, PG, PG, MRK, MRK, MRK, MCD, MCD, MCD, KO, KO, KO, JNJ, JNJ, JNJ, IBM, IBM, IBM, CVX, CVX, CVX, CSCO, CSCO, CSCO, AMGN, VZ</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -1760,7 +1760,7 @@
     <col width="19" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
     <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="21" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
     <col width="23" customWidth="1" min="11" max="11"/>
     <col width="30" customWidth="1" min="12" max="12"/>
     <col width="24" customWidth="1" min="13" max="13"/>
@@ -1884,16 +1884,16 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1506</v>
+        <v>0.1512</v>
       </c>
       <c r="K2" t="n">
-        <v>1.004</v>
+        <v>1.008</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
     </row>
     <row r="3">
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20.08</v>
+        <v>20.16</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>

</xml_diff>